<commit_message>
added new examples to validate
</commit_message>
<xml_diff>
--- a/docs/us-core-device.xlsx
+++ b/docs/us-core-device.xlsx
@@ -457,6 +457,9 @@
     <t>The device identifier (DI) is a mandatory, fixed portion of a UDI that identifies the labeler and the specific version or model of a device.</t>
   </si>
   <si>
+    <t>NA (not Supoorted)</t>
+  </si>
+  <si>
     <t>Role.id.extension</t>
   </si>
   <si>
@@ -534,9 +537,6 @@
   </si>
   <si>
     <t>The AIDC form of UDIs should be scanned or otherwise used for the identification of the device whenever possible to minimize errors in records resulting from manual transcriptions. If separate barcodes for DI and PI are present, concatenate the string with DI first and in order of human readable expression on label.</t>
-  </si>
-  <si>
-    <t>NA (not Supoorted)</t>
   </si>
   <si>
     <t>A unique device identifier (UDI) on a device label a form that uses automatic identification and data capture (AIDC) technology.</t>
@@ -3050,7 +3050,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>136</v>
       </c>
@@ -3060,13 +3060,13 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s" s="2">
         <v>47</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>40</v>
@@ -3147,25 +3147,25 @@
         <v>40</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3187,10 +3187,10 @@
         <v>60</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3241,7 +3241,7 @@
         <v>40</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>41</v>
@@ -3259,18 +3259,18 @@
         <v>40</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3296,14 +3296,14 @@
         <v>60</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>40</v>
@@ -3352,7 +3352,7 @@
         <v>40</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>41</v>
@@ -3370,7 +3370,7 @@
         <v>40</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>40</v>
@@ -3381,11 +3381,11 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3404,16 +3404,16 @@
         <v>48</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3463,7 +3463,7 @@
         <v>40</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>41</v>
@@ -3478,10 +3478,10 @@
         <v>40</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>40</v>
@@ -3592,7 +3592,7 @@
         <v>120</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>40</v>
@@ -4037,7 +4037,7 @@
         <v>196</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>197</v>
@@ -4146,13 +4146,13 @@
         <v>201</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>89</v>
       </c>
     </row>
-    <row r="27" hidden="true">
+    <row r="27">
       <c r="A27" t="s" s="2">
         <v>202</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>47</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>40</v>
@@ -4249,19 +4249,19 @@
         <v>40</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>206</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>207</v>
       </c>
     </row>
-    <row r="28" hidden="true">
+    <row r="28">
       <c r="A28" t="s" s="2">
         <v>208</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>47</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>40</v>
@@ -4358,19 +4358,19 @@
         <v>40</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>211</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>212</v>
       </c>
     </row>
-    <row r="29" hidden="true">
+    <row r="29">
       <c r="A29" t="s" s="2">
         <v>213</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>47</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>40</v>
@@ -4467,19 +4467,19 @@
         <v>40</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>196</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM29" t="s" s="2">
         <v>197</v>
       </c>
     </row>
-    <row r="30" hidden="true">
+    <row r="30">
       <c r="A30" t="s" s="2">
         <v>216</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>47</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>40</v>
@@ -4578,13 +4578,13 @@
         <v>40</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>220</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>40</v>
@@ -5244,7 +5244,7 @@
         <v>236</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>40</v>
@@ -5353,7 +5353,7 @@
         <v>240</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>40</v>
@@ -5464,7 +5464,7 @@
         <v>220</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>40</v>
@@ -6233,7 +6233,7 @@
         <v>40</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>40</v>
@@ -6893,7 +6893,7 @@
         <v>40</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>40</v>

</xml_diff>